<commit_message>
Fix attribute elements for EML
</commit_message>
<xml_diff>
--- a/data-raw/Metadata/Environmentals - Metadata.xlsx
+++ b/data-raw/Metadata/Environmentals - Metadata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cory Starr\Desktop\EDI\Metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\data-stewardship\EDI_data_repos_to_upload\stanislaus_rst_edi\data-raw\Metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD0D15F-3A39-4380-858B-800E9D3348D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14325" windowHeight="10740" tabRatio="834"/>
+    <workbookView xWindow="-3300" yWindow="-14040" windowWidth="20460" windowHeight="10920" tabRatio="834" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -26,16 +27,11 @@
     <sheet name="code_definitions" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="110">
   <si>
     <t>first_name</t>
   </si>
@@ -331,18 +327,6 @@
     <t>text</t>
   </si>
   <si>
-    <t>meters per second (m/s)</t>
-  </si>
-  <si>
-    <t>nephelometric turbidity units (NTU)</t>
-  </si>
-  <si>
-    <t>milligrams per liter (mg/L)</t>
-  </si>
-  <si>
-    <t>centimeters (cm)</t>
-  </si>
-  <si>
     <t>Juvenile Salmonid Emigration Monitoring in the Stanislaus River at Caswell Memorial State Park, California.</t>
   </si>
   <si>
@@ -363,11 +347,26 @@
   <si>
     <t>CVPIA</t>
   </si>
+  <si>
+    <t xml:space="preserve">nephelometric turbidity units </t>
+  </si>
+  <si>
+    <t>meterPerSecond</t>
+  </si>
+  <si>
+    <t>milligramPerLiter</t>
+  </si>
+  <si>
+    <t>centimeter</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -425,7 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -459,6 +458,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -842,10 +844,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -874,10 +876,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>" Point, LineString, LinearRing, Polygon, Multipoint, MultiLineString, MultiPolygon, MultiGeometry"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"tabular, vector, raster"</formula1>
     </dataValidation>
   </dataValidations>
@@ -886,7 +888,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -935,7 +937,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>"chinook, steelhead, delta_smelt, white_sturgeon, green_sturgeon"</formula1>
     </dataValidation>
   </dataValidations>
@@ -945,10 +947,12 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AMG10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1044,7 +1048,7 @@
         <v>96</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
@@ -1061,7 +1065,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -1077,8 +1081,8 @@
       <c r="F5" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>99</v>
+      <c r="G5" s="18" t="s">
+        <v>105</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>95</v>
@@ -1106,8 +1110,8 @@
       <c r="F6" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>98</v>
+      <c r="G6" s="18" t="s">
+        <v>106</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>95</v>
@@ -1135,8 +1139,8 @@
       <c r="F7" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>100</v>
+      <c r="G7" s="18" t="s">
+        <v>107</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>95</v>
@@ -1164,8 +1168,8 @@
       <c r="F8" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>101</v>
+      <c r="G8" s="18" t="s">
+        <v>108</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>95</v>
@@ -1196,19 +1200,19 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1021">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1021" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1021">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1021" xr:uid="{00000000-0002-0000-0A00-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1021">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1021" xr:uid="{00000000-0002-0000-0A00-000002000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0A00-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1218,7 +1222,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -1249,10 +1253,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1309,7 +1315,7 @@
         <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="E3" t="s">
         <v>68</v>
@@ -1317,7 +1323,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1005">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1005" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"creator,field technician,program founder,other,associate,reviewer,researcher,principal investigator,lab technician"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1328,7 +1334,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -1349,10 +1355,10 @@
     </row>
     <row r="2" spans="1:2" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1362,7 +1368,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -1383,12 +1389,12 @@
     </row>
     <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1403,7 +1409,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1413,7 +1419,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -1446,12 +1452,12 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"CCO, CCBY"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1461,7 +1467,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1497,7 +1503,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"creator,field technician,program founder,other,associate,reviewer,researcher,principal investigator,lab technician"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1507,7 +1513,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -1554,7 +1560,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please check default funding values from dropdown menu before manually adding funding information _x000a_" sqref="A1:A1048576">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please check default funding values from dropdown menu before manually adding funding information _x000a_" sqref="A1:A1048576" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>"USBR, CDWR, CDFW"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1564,7 +1570,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -1592,14 +1598,14 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A38:A1002">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A38:A1002" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>"completed,ongoing"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>"daily, weekly, monthly, annually"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A37" xr:uid="{00000000-0002-0000-0700-000002000000}">
       <formula1>"complete, ongoing "</formula1>
     </dataValidation>
   </dataValidations>
@@ -1609,7 +1615,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -1649,7 +1655,7 @@
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B2" s="2">
         <v>-121.179152</v>
@@ -1690,7 +1696,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G8">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G8" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>F2</formula1>
     </dataValidation>
   </dataValidations>
@@ -1700,12 +1706,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1714,7 +1714,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010062F3A0D97C24D44188E22ED6BF629E5F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d417724eab557a4a1613df09cf549db5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0babd99f-cddb-4efe-bfbd-78b0de5d1c16" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="452ce7caafae2949ffe48c11a29016ca" ns2:_="">
     <xsd:import namespace="0babd99f-cddb-4efe-bfbd-78b0de5d1c16"/>
@@ -1904,23 +1904,13 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A4324EA-0DD5-429A-A6A3-8853D3F17487}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0babd99f-cddb-4efe-bfbd-78b0de5d1c16"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7069DB4E-2E54-4EC8-AFE1-B50A3BCE1246}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1928,7 +1918,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B1783C-B3FB-44F3-8C80-B8883BF74C35}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1944,4 +1934,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A4324EA-0DD5-429A-A6A3-8853D3F17487}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0babd99f-cddb-4efe-bfbd-78b0de5d1c16"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to github url
</commit_message>
<xml_diff>
--- a/data-raw/Metadata/Environmentals - Metadata.xlsx
+++ b/data-raw/Metadata/Environmentals - Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\data-stewardship\EDI_data_repos_to_upload\stanislaus_rst_edi\data-raw\Metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD0D15F-3A39-4380-858B-800E9D3348D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2AE56D-4D2C-4BFB-A713-93A8AA8B42A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3300" yWindow="-14040" windowWidth="20460" windowHeight="10920" tabRatio="834" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18735" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="834" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -26,12 +26,21 @@
     <sheet name="attribute" sheetId="9" r:id="rId11"/>
     <sheet name="code_definitions" sheetId="10" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="111">
   <si>
     <t>first_name</t>
   </si>
@@ -246,9 +255,6 @@
     <t>Rotary Screw Traps</t>
   </si>
   <si>
-    <t>Central Valley Project Improvement Act (CVPIA)</t>
-  </si>
-  <si>
     <t xml:space="preserve">ongoing </t>
   </si>
   <si>
@@ -361,13 +367,19 @@
   </si>
   <si>
     <t>creator</t>
+  </si>
+  <si>
+    <t>Annual quantification of juvenile Chinook salmon production and the abundance of juvenile steelhead in the Stanislaus River using rotary screw traps</t>
+  </si>
+  <si>
+    <t>USBR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -389,6 +401,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -424,7 +442,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -462,6 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -868,7 +887,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
         <v>60</v>
@@ -1015,19 +1034,19 @@
     </row>
     <row r="2" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>91</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>92</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="14">
@@ -1039,53 +1058,53 @@
     </row>
     <row r="3" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>96</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>96</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="F5" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>95</v>
       </c>
       <c r="L5" s="10">
         <v>1.01</v>
@@ -1096,25 +1115,25 @@
     </row>
     <row r="6" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="F6" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>95</v>
       </c>
       <c r="L6" s="10">
         <v>0.1</v>
@@ -1125,25 +1144,25 @@
     </row>
     <row r="7" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="F7" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>95</v>
       </c>
       <c r="L7" s="10">
         <v>2.31</v>
@@ -1154,25 +1173,25 @@
     </row>
     <row r="8" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="F8" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>95</v>
       </c>
       <c r="L8" s="10">
         <v>60</v>
@@ -1183,16 +1202,16 @@
     </row>
     <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>96</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1256,7 +1275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1315,7 +1334,7 @@
         <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E3" t="s">
         <v>68</v>
@@ -1355,10 +1374,10 @@
     </row>
     <row r="2" spans="1:2" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>98</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1389,12 +1408,12 @@
     </row>
     <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1409,7 +1428,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1452,7 +1471,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1516,7 +1535,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1548,13 +1569,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="2"/>
+      <c r="D2" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
@@ -1590,10 +1613,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1655,7 +1678,7 @@
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="2">
         <v>-121.179152</v>
@@ -1706,12 +1729,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1905,15 +1925,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7069DB4E-2E54-4EC8-AFE1-B50A3BCE1246}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A4324EA-0DD5-429A-A6A3-8853D3F17487}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0babd99f-cddb-4efe-bfbd-78b0de5d1c16"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1937,17 +1968,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A4324EA-0DD5-429A-A6A3-8853D3F17487}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7069DB4E-2E54-4EC8-AFE1-B50A3BCE1246}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0babd99f-cddb-4efe-bfbd-78b0de5d1c16"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adds updated data from logan
</commit_message>
<xml_diff>
--- a/data-raw/Metadata/Environmentals - Metadata.xlsx
+++ b/data-raw/Metadata/Environmentals - Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\data-stewardship\EDI_data_repos_to_upload\stanislaus_rst_edi\data-raw\Metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2AE56D-4D2C-4BFB-A713-93A8AA8B42A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54089EB9-8223-4DDB-9365-2D6A6758A3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18735" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="834" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="90" windowWidth="9960" windowHeight="7875" tabRatio="834" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="222">
   <si>
     <t>first_name</t>
   </si>
@@ -228,15 +228,6 @@
     <t>researcher</t>
   </si>
   <si>
-    <t>Cory</t>
-  </si>
-  <si>
-    <t>Starr</t>
-  </si>
-  <si>
-    <t>cstarr@psmfc.org</t>
-  </si>
-  <si>
     <t>Logan</t>
   </si>
   <si>
@@ -373,6 +364,348 @@
   </si>
   <si>
     <t>USBR</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>Galinat</t>
+  </si>
+  <si>
+    <t>agalinat@psmfc.org</t>
+  </si>
+  <si>
+    <t>chinook</t>
+  </si>
+  <si>
+    <t>steelhead</t>
+  </si>
+  <si>
+    <t>Bigscale logperch</t>
+  </si>
+  <si>
+    <t>Animalia</t>
+  </si>
+  <si>
+    <t>Chordata</t>
+  </si>
+  <si>
+    <t>Actinopterygii</t>
+  </si>
+  <si>
+    <t>Perciformes</t>
+  </si>
+  <si>
+    <t>Percidae</t>
+  </si>
+  <si>
+    <t>Percina</t>
+  </si>
+  <si>
+    <t>macrolepida</t>
+  </si>
+  <si>
+    <t>Black crappie</t>
+  </si>
+  <si>
+    <t>Centrarchidae</t>
+  </si>
+  <si>
+    <t>Pomoxis</t>
+  </si>
+  <si>
+    <t>nigromaculatus</t>
+  </si>
+  <si>
+    <t>Bluegill</t>
+  </si>
+  <si>
+    <t>Lepomis</t>
+  </si>
+  <si>
+    <t>macrochirus</t>
+  </si>
+  <si>
+    <t>Brown bullhead</t>
+  </si>
+  <si>
+    <t>Siluriformes</t>
+  </si>
+  <si>
+    <t>Ictaluridae</t>
+  </si>
+  <si>
+    <t>Ameiurus</t>
+  </si>
+  <si>
+    <t>nabulosus</t>
+  </si>
+  <si>
+    <t>Channel catfish</t>
+  </si>
+  <si>
+    <t>Ictalurus punctatus</t>
+  </si>
+  <si>
+    <t>Fathead minnow</t>
+  </si>
+  <si>
+    <t>Cypriniformes</t>
+  </si>
+  <si>
+    <t>Cyprinidae</t>
+  </si>
+  <si>
+    <t>Pimephales</t>
+  </si>
+  <si>
+    <t>promelas</t>
+  </si>
+  <si>
+    <t>Golden shiner</t>
+  </si>
+  <si>
+    <t>Notemigonus</t>
+  </si>
+  <si>
+    <t>crysoleucas</t>
+  </si>
+  <si>
+    <t>Goldfish</t>
+  </si>
+  <si>
+    <t>Carassius</t>
+  </si>
+  <si>
+    <t>auratus</t>
+  </si>
+  <si>
+    <t>Green sunfish</t>
+  </si>
+  <si>
+    <t>cyanellus</t>
+  </si>
+  <si>
+    <t>Hardhead</t>
+  </si>
+  <si>
+    <t>Mylopharodon</t>
+  </si>
+  <si>
+    <t>conocephalus</t>
+  </si>
+  <si>
+    <t>Inland silverside</t>
+  </si>
+  <si>
+    <t>Atheriniformes</t>
+  </si>
+  <si>
+    <t>Atherinopsidae</t>
+  </si>
+  <si>
+    <t>Menidia</t>
+  </si>
+  <si>
+    <t>beryllina</t>
+  </si>
+  <si>
+    <t>Largemouth bass</t>
+  </si>
+  <si>
+    <t>Micropterus</t>
+  </si>
+  <si>
+    <t>salmoides</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Pacific lamprey</t>
+  </si>
+  <si>
+    <t>Cephalaspidomorphi</t>
+  </si>
+  <si>
+    <t>Petromyzontiformes</t>
+  </si>
+  <si>
+    <t>Petromyzontidae</t>
+  </si>
+  <si>
+    <t>Entosphenus</t>
+  </si>
+  <si>
+    <t>Tridentata</t>
+  </si>
+  <si>
+    <t>Prickly sculpin</t>
+  </si>
+  <si>
+    <t>Scorpaeniformes</t>
+  </si>
+  <si>
+    <t>Cottidae</t>
+  </si>
+  <si>
+    <t>Cottus</t>
+  </si>
+  <si>
+    <t>asper</t>
+  </si>
+  <si>
+    <t>Redear sunfish</t>
+  </si>
+  <si>
+    <t>microlophus</t>
+  </si>
+  <si>
+    <t>Riffle sculpin</t>
+  </si>
+  <si>
+    <t>gulosus</t>
+  </si>
+  <si>
+    <t>Sacramento pikeminnow</t>
+  </si>
+  <si>
+    <t>Ptychocheilus</t>
+  </si>
+  <si>
+    <t>grandis</t>
+  </si>
+  <si>
+    <t>Sacramento sucker</t>
+  </si>
+  <si>
+    <t>Catostomidae</t>
+  </si>
+  <si>
+    <t>Catostomus</t>
+  </si>
+  <si>
+    <t>occidentalis</t>
+  </si>
+  <si>
+    <t>Smallmouth bass</t>
+  </si>
+  <si>
+    <t>dolomieu</t>
+  </si>
+  <si>
+    <t>Speckled dace</t>
+  </si>
+  <si>
+    <t>Rhinichthys</t>
+  </si>
+  <si>
+    <t>osculus</t>
+  </si>
+  <si>
+    <t>Spotted bass</t>
+  </si>
+  <si>
+    <t>punctulatus</t>
+  </si>
+  <si>
+    <t>Sucker</t>
+  </si>
+  <si>
+    <t>Threadfin shad</t>
+  </si>
+  <si>
+    <t>Clupeiformes</t>
+  </si>
+  <si>
+    <t>Clupeidae</t>
+  </si>
+  <si>
+    <t>Dorosoma</t>
+  </si>
+  <si>
+    <t>petenense</t>
+  </si>
+  <si>
+    <t>Tule perch</t>
+  </si>
+  <si>
+    <t>Embiotocidae</t>
+  </si>
+  <si>
+    <t>Hysterocarpus</t>
+  </si>
+  <si>
+    <t>traskii</t>
+  </si>
+  <si>
+    <t>Unknown bass (Micropterus)</t>
+  </si>
+  <si>
+    <t>Unknown bony fish</t>
+  </si>
+  <si>
+    <t>Unknown catfish or bullhead</t>
+  </si>
+  <si>
+    <t>Unknown Centrarchid</t>
+  </si>
+  <si>
+    <t>Unknown lamprey (Entosphenus or Lampetra)</t>
+  </si>
+  <si>
+    <t>Unknown minnow</t>
+  </si>
+  <si>
+    <t>Unknown sculpin (Cottus)</t>
+  </si>
+  <si>
+    <t>Unknown sunfish (Lepomis)</t>
+  </si>
+  <si>
+    <t>Wakasagi</t>
+  </si>
+  <si>
+    <t>Osmeriformes</t>
+  </si>
+  <si>
+    <t>Osmeridae</t>
+  </si>
+  <si>
+    <t>Hypomesus</t>
+  </si>
+  <si>
+    <t>nipponensis</t>
+  </si>
+  <si>
+    <t>Warmouth</t>
+  </si>
+  <si>
+    <t>Western mosquitofish</t>
+  </si>
+  <si>
+    <t>Cyprinodontiformes</t>
+  </si>
+  <si>
+    <t>Poeciliidae</t>
+  </si>
+  <si>
+    <t>Gambusia</t>
+  </si>
+  <si>
+    <t>affinis</t>
+  </si>
+  <si>
+    <t>White catfish</t>
+  </si>
+  <si>
+    <t>catus</t>
+  </si>
+  <si>
+    <t>White crappie</t>
+  </si>
+  <si>
+    <t>annularis</t>
   </si>
 </sst>
 </file>
@@ -887,7 +1220,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
         <v>60</v>
@@ -908,9 +1241,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -952,6 +1287,1046 @@
       </c>
       <c r="J1" s="11" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="11">
+        <v>168487</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="J5" s="11">
+        <v>168167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J6" s="11">
+        <v>168141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="J7" s="11">
+        <v>164043</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="J8" s="11">
+        <v>163998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="J9" s="11">
+        <v>163517</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="J10" s="11">
+        <v>163368</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="J11" s="11">
+        <v>163350</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J12" s="11">
+        <v>168132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="J13" s="11">
+        <v>163587</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="J14" s="11">
+        <v>165993</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="J15" s="11">
+        <v>168160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="J16" s="11">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="J17" s="11">
+        <v>159698</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J18" s="11">
+        <v>167233</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="J19" s="11">
+        <v>168154</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="J20" s="11">
+        <v>167234</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="J21" s="11">
+        <v>163524</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="J22" s="11">
+        <v>163908</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="J23" s="11">
+        <v>550562</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="J24" s="11">
+        <v>163387</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="J25" s="11">
+        <v>168161</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="J26" s="11">
+        <v>163892</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="J27" s="11">
+        <v>161738</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="J28" s="11">
+        <v>553322</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="J29" s="11">
+        <v>168158</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J30" s="11">
+        <v>161030</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="J31" s="11">
+        <v>163995</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J32" s="11">
+        <v>168093</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="J33" s="11">
+        <v>159697</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="J34" s="11">
+        <v>163342</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="J35" s="11">
+        <v>167229</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="J36" s="11">
+        <v>168130</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="J37" s="11">
+        <v>162033</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="J38" s="11">
+        <v>168139</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="J39" s="11">
+        <v>165878</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="J40" s="11">
+        <v>164037</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="J41" s="11">
+        <v>168166</v>
       </c>
     </row>
   </sheetData>
@@ -1034,19 +2409,19 @@
     </row>
     <row r="2" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="14">
@@ -1058,53 +2433,53 @@
     </row>
     <row r="3" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L5" s="10">
         <v>1.01</v>
@@ -1115,25 +2490,25 @@
     </row>
     <row r="6" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L6" s="10">
         <v>0.1</v>
@@ -1144,25 +2519,25 @@
     </row>
     <row r="7" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L7" s="10">
         <v>2.31</v>
@@ -1173,25 +2548,25 @@
     </row>
     <row r="8" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L8" s="10">
         <v>60</v>
@@ -1202,16 +2577,16 @@
     </row>
     <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1244,7 +2619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1276,7 +2651,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1308,36 +2683,36 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
         <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" t="s">
         <v>65</v>
-      </c>
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E3" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1356,7 +2731,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1374,10 +2751,10 @@
     </row>
     <row r="2" spans="1:2" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1408,27 +2785,27 @@
     </row>
     <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1471,7 +2848,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1535,7 +2912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1571,12 +2948,12 @@
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="10"/>
       <c r="D2" s="19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -1613,10 +2990,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1641,7 +3018,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1678,7 +3057,7 @@
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B2" s="2">
         <v>-121.179152</v>
@@ -1696,7 +3075,7 @@
         <v>42767</v>
       </c>
       <c r="G2" s="5">
-        <v>43973</v>
+        <v>44350</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1729,12 +3108,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010062F3A0D97C24D44188E22ED6BF629E5F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d417724eab557a4a1613df09cf549db5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0babd99f-cddb-4efe-bfbd-78b0de5d1c16" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="452ce7caafae2949ffe48c11a29016ca" ns2:_="">
     <xsd:import namespace="0babd99f-cddb-4efe-bfbd-78b0de5d1c16"/>
@@ -1924,6 +3297,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1934,22 +3313,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A4324EA-0DD5-429A-A6A3-8853D3F17487}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0babd99f-cddb-4efe-bfbd-78b0de5d1c16"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B1783C-B3FB-44F3-8C80-B8883BF74C35}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1967,6 +3330,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A4324EA-0DD5-429A-A6A3-8853D3F17487}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0babd99f-cddb-4efe-bfbd-78b0de5d1c16"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7069DB4E-2E54-4EC8-AFE1-B50A3BCE1246}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Adds version 2 files that are on EDI
</commit_message>
<xml_diff>
--- a/data-raw/Metadata/Environmentals - Metadata.xlsx
+++ b/data-raw/Metadata/Environmentals - Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\data-stewardship\EDI_data_repos_to_upload\stanislaus_rst_edi\data-raw\Metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54089EB9-8223-4DDB-9365-2D6A6758A3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A994EDF-8DAC-4644-AD54-2701C9238DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="90" windowWidth="9960" windowHeight="7875" tabRatio="834" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="90" windowWidth="20025" windowHeight="7875" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -327,9 +327,6 @@
     <t>Juvenile Salmonid Emigration Monitoring in the Stanislaus River at Caswell Memorial State Park, California.</t>
   </si>
   <si>
-    <t>Stanislaus River at Caswell Memorial State Park RST data (2017 - 2020)</t>
-  </si>
-  <si>
     <t>Stanislaus River</t>
   </si>
   <si>
@@ -706,6 +703,9 @@
   </si>
   <si>
     <t>annularis</t>
+  </si>
+  <si>
+    <t>Stanislaus River at Caswell Memorial State Park RST data (2017 - 2021)</t>
   </si>
 </sst>
 </file>
@@ -1199,7 +1199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1291,38 +1291,38 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E4" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="H4" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="J4" s="11">
         <v>168487</v>
@@ -1330,28 +1330,28 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="H5" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>123</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>124</v>
       </c>
       <c r="J5" s="11">
         <v>168167</v>
@@ -1359,28 +1359,28 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>126</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="J6" s="11">
         <v>168141</v>
@@ -1388,28 +1388,28 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" s="11" t="s">
+      <c r="G7" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="H7" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="I7" s="11" t="s">
         <v>131</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>132</v>
       </c>
       <c r="J7" s="11">
         <v>164043</v>
@@ -1417,28 +1417,28 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>134</v>
-      </c>
       <c r="I8" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J8" s="11">
         <v>163998</v>
@@ -1446,28 +1446,28 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F9" s="11" t="s">
+      <c r="G9" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="H9" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>138</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>139</v>
       </c>
       <c r="J9" s="11">
         <v>163517</v>
@@ -1475,28 +1475,28 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H10" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="H10" s="11" t="s">
+      <c r="I10" s="11" t="s">
         <v>141</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>142</v>
       </c>
       <c r="J10" s="11">
         <v>163368</v>
@@ -1504,28 +1504,28 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="H11" s="11" t="s">
+      <c r="I11" s="11" t="s">
         <v>144</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>145</v>
       </c>
       <c r="J11" s="11">
         <v>163350</v>
@@ -1533,28 +1533,28 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="I12" s="11" t="s">
         <v>146</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>147</v>
       </c>
       <c r="J12" s="11">
         <v>168132</v>
@@ -1562,28 +1562,28 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H13" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="H13" s="11" t="s">
+      <c r="I13" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>150</v>
       </c>
       <c r="J13" s="11">
         <v>163587</v>
@@ -1591,28 +1591,28 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F14" s="11" t="s">
+      <c r="G14" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="H14" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="I14" s="11" t="s">
         <v>154</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>155</v>
       </c>
       <c r="J14" s="11">
         <v>165993</v>
@@ -1620,28 +1620,28 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H15" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="H15" s="11" t="s">
+      <c r="I15" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>158</v>
       </c>
       <c r="J15" s="11">
         <v>168160</v>
@@ -1649,7 +1649,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J16" s="11">
         <v>250</v>
@@ -1657,28 +1657,28 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="G17" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="H17" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="I17" s="11" t="s">
         <v>164</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>165</v>
       </c>
       <c r="J17" s="11">
         <v>159698</v>
@@ -1686,28 +1686,28 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F18" s="11" t="s">
+      <c r="G18" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="H18" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="I18" s="11" t="s">
         <v>169</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>170</v>
       </c>
       <c r="J18" s="11">
         <v>167233</v>
@@ -1715,28 +1715,28 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="I19" s="11" t="s">
         <v>171</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>172</v>
       </c>
       <c r="J19" s="11">
         <v>168154</v>
@@ -1744,28 +1744,28 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="I20" s="11" t="s">
         <v>173</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>174</v>
       </c>
       <c r="J20" s="11">
         <v>167234</v>
@@ -1773,28 +1773,28 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H21" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="H21" s="11" t="s">
+      <c r="I21" s="11" t="s">
         <v>176</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>177</v>
       </c>
       <c r="J21" s="11">
         <v>163524</v>
@@ -1802,28 +1802,28 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G22" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="G22" s="11" t="s">
+      <c r="H22" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="I22" s="11" t="s">
         <v>180</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>181</v>
       </c>
       <c r="J22" s="11">
         <v>163908</v>
@@ -1831,28 +1831,28 @@
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="I23" s="11" t="s">
         <v>182</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>183</v>
       </c>
       <c r="J23" s="11">
         <v>550562</v>
@@ -1860,28 +1860,28 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H24" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="H24" s="11" t="s">
+      <c r="I24" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>186</v>
       </c>
       <c r="J24" s="11">
         <v>163387</v>
@@ -1889,28 +1889,28 @@
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="I25" s="11" t="s">
         <v>187</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>188</v>
       </c>
       <c r="J25" s="11">
         <v>168161</v>
@@ -1918,22 +1918,22 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J26" s="11">
         <v>163892</v>
@@ -1941,28 +1941,28 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F27" s="11" t="s">
+      <c r="G27" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="H27" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="I27" s="11" t="s">
         <v>193</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>194</v>
       </c>
       <c r="J27" s="11">
         <v>161738</v>
@@ -1970,28 +1970,28 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G28" s="11" t="s">
+      <c r="H28" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="I28" s="11" t="s">
         <v>197</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>198</v>
       </c>
       <c r="J28" s="11">
         <v>553322</v>
@@ -1999,25 +1999,25 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E29" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="11" t="s">
-        <v>117</v>
-      </c>
       <c r="G29" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J29" s="11">
         <v>168158</v>
@@ -2025,16 +2025,16 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J30" s="11">
         <v>161030</v>
@@ -2042,22 +2042,22 @@
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F31" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="G31" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>130</v>
       </c>
       <c r="J31" s="11">
         <v>163995</v>
@@ -2065,22 +2065,22 @@
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E32" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F32" s="11" t="s">
-        <v>117</v>
-      </c>
       <c r="G32" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J32" s="11">
         <v>168093</v>
@@ -2088,22 +2088,22 @@
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E33" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="F33" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="G33" s="11" t="s">
         <v>162</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>163</v>
       </c>
       <c r="J33" s="11">
         <v>159697</v>
@@ -2111,22 +2111,22 @@
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F34" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G34" s="11" t="s">
         <v>136</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>137</v>
       </c>
       <c r="J34" s="11">
         <v>163342</v>
@@ -2134,25 +2134,25 @@
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F35" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G35" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="H35" s="11" t="s">
         <v>168</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>169</v>
       </c>
       <c r="J35" s="11">
         <v>167229</v>
@@ -2160,25 +2160,25 @@
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E36" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F36" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F36" s="11" t="s">
-        <v>117</v>
-      </c>
       <c r="G36" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J36" s="11">
         <v>168130</v>
@@ -2186,28 +2186,28 @@
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F37" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F37" s="11" t="s">
+      <c r="G37" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="G37" s="11" t="s">
+      <c r="H37" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="I37" s="11" t="s">
         <v>210</v>
-      </c>
-      <c r="I37" s="11" t="s">
-        <v>211</v>
       </c>
       <c r="J37" s="11">
         <v>162033</v>
@@ -2215,28 +2215,28 @@
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E38" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F38" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F38" s="11" t="s">
-        <v>117</v>
-      </c>
       <c r="G38" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J38" s="11">
         <v>168139</v>
@@ -2244,28 +2244,28 @@
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="C39" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F39" s="11" t="s">
+      <c r="G39" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="H39" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="H39" s="11" t="s">
+      <c r="I39" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="J39" s="11">
         <v>165878</v>
@@ -2273,28 +2273,28 @@
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="I40" s="11" t="s">
         <v>218</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>219</v>
       </c>
       <c r="J40" s="11">
         <v>164037</v>
@@ -2302,28 +2302,28 @@
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="I41" s="11" t="s">
         <v>220</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="I41" s="11" t="s">
-        <v>221</v>
       </c>
       <c r="J41" s="11">
         <v>168166</v>
@@ -2476,7 +2476,7 @@
         <v>89</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>91</v>
@@ -2505,7 +2505,7 @@
         <v>89</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>91</v>
@@ -2534,7 +2534,7 @@
         <v>89</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>91</v>
@@ -2563,7 +2563,7 @@
         <v>89</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>91</v>
@@ -2619,7 +2619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2683,13 +2683,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
         <v>108</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="D2" t="s">
         <v>61</v>
@@ -2709,7 +2709,7 @@
         <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E3" t="s">
         <v>65</v>
@@ -2754,7 +2754,7 @@
         <v>94</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>95</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2785,12 +2785,12 @@
     </row>
     <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2805,7 +2805,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2848,7 +2848,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2948,12 +2948,12 @@
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="10"/>
       <c r="D2" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -3057,7 +3057,7 @@
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="2">
         <v>-121.179152</v>
@@ -3108,6 +3108,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010062F3A0D97C24D44188E22ED6BF629E5F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d417724eab557a4a1613df09cf549db5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0babd99f-cddb-4efe-bfbd-78b0de5d1c16" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="452ce7caafae2949ffe48c11a29016ca" ns2:_="">
     <xsd:import namespace="0babd99f-cddb-4efe-bfbd-78b0de5d1c16"/>
@@ -3297,12 +3303,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3313,6 +3313,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A4324EA-0DD5-429A-A6A3-8853D3F17487}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0babd99f-cddb-4efe-bfbd-78b0de5d1c16"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B1783C-B3FB-44F3-8C80-B8883BF74C35}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3330,22 +3346,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A4324EA-0DD5-429A-A6A3-8853D3F17487}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0babd99f-cddb-4efe-bfbd-78b0de5d1c16"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7069DB4E-2E54-4EC8-AFE1-B50A3BCE1246}">
   <ds:schemaRefs>

</xml_diff>